<commit_message>
update 18/05 aluguel carro e moto
</commit_message>
<xml_diff>
--- a/public/Relatorio_ConfigMotos.xlsx
+++ b/public/Relatorio_ConfigMotos.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>nome</t>
   </si>
@@ -28,9 +28,6 @@
     <t>cor</t>
   </si>
   <si>
-    <t>nome_dono</t>
-  </si>
-  <si>
     <t>observacoes</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
     <t>Data de Cadastro</t>
   </si>
   <si>
+    <t>Valor diaria</t>
+  </si>
+  <si>
     <t>Yamaha MT-07</t>
   </si>
   <si>
@@ -52,16 +52,13 @@
     <t>preto</t>
   </si>
   <si>
-    <t>Matheus</t>
-  </si>
-  <si>
     <t>teste</t>
   </si>
   <si>
     <t>Ativo</t>
   </si>
   <si>
-    <t>2024-05-17 16:22:23</t>
+    <t>2024-05-18 23:22:37</t>
   </si>
 </sst>
 </file>
@@ -448,17 +445,17 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>80000</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2">
-        <v>15000</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="H2">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update adição de compra carro/moto, correção de bugs no aluguel de ambos.
</commit_message>
<xml_diff>
--- a/public/Relatorio_ConfigMotos.xlsx
+++ b/public/Relatorio_ConfigMotos.xlsx
@@ -10,16 +10,16 @@
     <sheet name="ConfigMotos" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ConfigMotos'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ConfigMotos'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
-  <si>
-    <t>nome</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+  <si>
+    <t>modelo</t>
   </si>
   <si>
     <t>marca</t>
@@ -28,10 +28,16 @@
     <t>cor</t>
   </si>
   <si>
+    <t>placa</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
     <t>observacoes</t>
   </si>
   <si>
-    <t>valor_compra</t>
+    <t>valor de compra</t>
   </si>
   <si>
     <t>status</t>
@@ -43,7 +49,7 @@
     <t>Valor diaria</t>
   </si>
   <si>
-    <t>Yamaha MT-07</t>
+    <t>Yamaha i8</t>
   </si>
   <si>
     <t>Yamaha</t>
@@ -52,13 +58,28 @@
     <t>preto</t>
   </si>
   <si>
+    <t>JDSA214</t>
+  </si>
+  <si>
     <t>teste</t>
   </si>
   <si>
     <t>Ativo</t>
   </si>
   <si>
-    <t>2024-05-18 23:22:37</t>
+    <t>2024-05-19 09:57:11</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Azul Metálico</t>
+  </si>
+  <si>
+    <t>tiue822</t>
+  </si>
+  <si>
+    <t>2024-05-19 10:23:20</t>
   </si>
 </sst>
 </file>
@@ -398,7 +419,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,35 +452,79 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>80000</v>
+        <v>2025</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2020</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>14000</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2"/>
+  <autoFilter ref="A1:J3"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>